<commit_message>
Complete loading capability of current railway od_pairs in operation.
</commit_message>
<xml_diff>
--- a/data/railway_paths.xlsx
+++ b/data/railway_paths.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" calcMode="manual"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7665" uniqueCount="3788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7743" uniqueCount="3838">
   <si>
     <t>id_od</t>
   </si>
@@ -11378,14 +11378,172 @@
   </si>
   <si>
     <t>No encontrada</t>
+  </si>
+  <si>
+    <t>78-21</t>
+  </si>
+  <si>
+    <t>66-21</t>
+  </si>
+  <si>
+    <t>83-21</t>
+  </si>
+  <si>
+    <t>64-21</t>
+  </si>
+  <si>
+    <t>67-21</t>
+  </si>
+  <si>
+    <t>62-21</t>
+  </si>
+  <si>
+    <t>49-45</t>
+  </si>
+  <si>
+    <t>63-21</t>
+  </si>
+  <si>
+    <t>51-45</t>
+  </si>
+  <si>
+    <t>49-21</t>
+  </si>
+  <si>
+    <t>56-21</t>
+  </si>
+  <si>
+    <t>72-21</t>
+  </si>
+  <si>
+    <t>59-21</t>
+  </si>
+  <si>
+    <t>52-45</t>
+  </si>
+  <si>
+    <t>29-21</t>
+  </si>
+  <si>
+    <t>27-21</t>
+  </si>
+  <si>
+    <t>32-21</t>
+  </si>
+  <si>
+    <t>60-21</t>
+  </si>
+  <si>
+    <t>28-21</t>
+  </si>
+  <si>
+    <t>58-21</t>
+  </si>
+  <si>
+    <t>25-21</t>
+  </si>
+  <si>
+    <t>26-21</t>
+  </si>
+  <si>
+    <t>57-21</t>
+  </si>
+  <si>
+    <t>46-45</t>
+  </si>
+  <si>
+    <t>23-21</t>
+  </si>
+  <si>
+    <t>24-21</t>
+  </si>
+  <si>
+    <t>078-083-1002-065-055-056-1004-021</t>
+  </si>
+  <si>
+    <t>066-067-014-015-017-021</t>
+  </si>
+  <si>
+    <t>083-064-063-014-057-021</t>
+  </si>
+  <si>
+    <t>064-063-014-057-021</t>
+  </si>
+  <si>
+    <t>067-014-015-017-021</t>
+  </si>
+  <si>
+    <t>049-051-1052-1037-046-1046-045</t>
+  </si>
+  <si>
+    <t>063-014-057-021</t>
+  </si>
+  <si>
+    <t>051-1052-1037-046-1046-045</t>
+  </si>
+  <si>
+    <t>049-095-1059-060-1023-023-021</t>
+  </si>
+  <si>
+    <t>056-058-020-019-021</t>
+  </si>
+  <si>
+    <t>059-058-020-019-021</t>
+  </si>
+  <si>
+    <t>052-1052-1037-046-1046-045</t>
+  </si>
+  <si>
+    <t>029-1023-023-021</t>
+  </si>
+  <si>
+    <t>027-007-026-025-024-1022-021</t>
+  </si>
+  <si>
+    <t>032-027-007-026-025-024-1022-021</t>
+  </si>
+  <si>
+    <t>060-1023-023-021</t>
+  </si>
+  <si>
+    <t>028-029-1023-023-021</t>
+  </si>
+  <si>
+    <t>058-020-019-021</t>
+  </si>
+  <si>
+    <t>025-024-1022-021</t>
+  </si>
+  <si>
+    <t>026-025-024-1022-021</t>
+  </si>
+  <si>
+    <t>057-021</t>
+  </si>
+  <si>
+    <t>046-1046-045</t>
+  </si>
+  <si>
+    <t>023-021</t>
+  </si>
+  <si>
+    <t>024-1022-021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -11413,9 +11571,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11717,11 +11877,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2555"/>
+  <dimension ref="A1:C2583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1208" workbookViewId="0">
-      <selection activeCell="C1220" sqref="C1220"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11731,13 +11889,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -39834,6 +39992,298 @@
       <c r="C2555" t="s">
         <v>3787</v>
       </c>
+    </row>
+    <row r="2556" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2556" s="1" t="s">
+        <v>3788</v>
+      </c>
+      <c r="B2556" t="s">
+        <v>3814</v>
+      </c>
+      <c r="C2556" t="s">
+        <v>3785</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2557" s="1" t="s">
+        <v>3789</v>
+      </c>
+      <c r="B2557" t="s">
+        <v>3815</v>
+      </c>
+      <c r="C2557" t="s">
+        <v>3785</v>
+      </c>
+    </row>
+    <row r="2558" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2558" s="1" t="s">
+        <v>3790</v>
+      </c>
+      <c r="B2558" t="s">
+        <v>3816</v>
+      </c>
+      <c r="C2558" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2559" s="1" t="s">
+        <v>3791</v>
+      </c>
+      <c r="B2559" t="s">
+        <v>3817</v>
+      </c>
+      <c r="C2559" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2560" s="1" t="s">
+        <v>3792</v>
+      </c>
+      <c r="B2560" t="s">
+        <v>3818</v>
+      </c>
+      <c r="C2560" t="s">
+        <v>3785</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2561" s="1" t="s">
+        <v>3793</v>
+      </c>
+      <c r="B2561" t="s">
+        <v>3783</v>
+      </c>
+      <c r="C2561" t="s">
+        <v>3787</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2562" s="1" t="s">
+        <v>3794</v>
+      </c>
+      <c r="B2562" t="s">
+        <v>3819</v>
+      </c>
+      <c r="C2562" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2563" s="1" t="s">
+        <v>3795</v>
+      </c>
+      <c r="B2563" t="s">
+        <v>3820</v>
+      </c>
+      <c r="C2563" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2564" s="1" t="s">
+        <v>3796</v>
+      </c>
+      <c r="B2564" t="s">
+        <v>3821</v>
+      </c>
+      <c r="C2564" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2565" s="1" t="s">
+        <v>3797</v>
+      </c>
+      <c r="B2565" t="s">
+        <v>3822</v>
+      </c>
+      <c r="C2565" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2566" s="1" t="s">
+        <v>3798</v>
+      </c>
+      <c r="B2566" t="s">
+        <v>3823</v>
+      </c>
+      <c r="C2566" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2567" s="1" t="s">
+        <v>3799</v>
+      </c>
+      <c r="B2567" t="s">
+        <v>3783</v>
+      </c>
+      <c r="C2567" t="s">
+        <v>3787</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2568" s="1" t="s">
+        <v>3800</v>
+      </c>
+      <c r="B2568" t="s">
+        <v>3824</v>
+      </c>
+      <c r="C2568" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2569" s="1" t="s">
+        <v>3801</v>
+      </c>
+      <c r="B2569" t="s">
+        <v>3825</v>
+      </c>
+      <c r="C2569" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2570" s="1" t="s">
+        <v>3802</v>
+      </c>
+      <c r="B2570" t="s">
+        <v>3826</v>
+      </c>
+      <c r="C2570" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2571" s="1" t="s">
+        <v>3803</v>
+      </c>
+      <c r="B2571" t="s">
+        <v>3827</v>
+      </c>
+      <c r="C2571" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2572" s="1" t="s">
+        <v>3804</v>
+      </c>
+      <c r="B2572" t="s">
+        <v>3828</v>
+      </c>
+      <c r="C2572" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2573" s="1" t="s">
+        <v>3805</v>
+      </c>
+      <c r="B2573" t="s">
+        <v>3829</v>
+      </c>
+      <c r="C2573" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2574" s="1" t="s">
+        <v>3806</v>
+      </c>
+      <c r="B2574" t="s">
+        <v>3830</v>
+      </c>
+      <c r="C2574" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2575" s="1" t="s">
+        <v>3807</v>
+      </c>
+      <c r="B2575" t="s">
+        <v>3831</v>
+      </c>
+      <c r="C2575" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2576" s="1" t="s">
+        <v>3808</v>
+      </c>
+      <c r="B2576" t="s">
+        <v>3832</v>
+      </c>
+      <c r="C2576" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2577" s="1" t="s">
+        <v>3809</v>
+      </c>
+      <c r="B2577" t="s">
+        <v>3833</v>
+      </c>
+      <c r="C2577" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2578" s="1" t="s">
+        <v>3810</v>
+      </c>
+      <c r="B2578" t="s">
+        <v>3834</v>
+      </c>
+      <c r="C2578" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2579" s="1" t="s">
+        <v>3811</v>
+      </c>
+      <c r="B2579" t="s">
+        <v>3835</v>
+      </c>
+      <c r="C2579" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2580" s="1" t="s">
+        <v>3812</v>
+      </c>
+      <c r="B2580" t="s">
+        <v>3836</v>
+      </c>
+      <c r="C2580" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2581" s="1" t="s">
+        <v>3813</v>
+      </c>
+      <c r="B2581" t="s">
+        <v>3837</v>
+      </c>
+      <c r="C2581" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2582"/>
+    </row>
+    <row r="2583" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2583"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix error in data.
</commit_message>
<xml_diff>
--- a/data/railway_paths.xlsx
+++ b/data/railway_paths.xlsx
@@ -18088,27 +18088,6 @@
     <t>021-023-1023-029-028</t>
   </si>
   <si>
-    <t>001-003-013-1012-011-070-071-073</t>
-  </si>
-  <si>
-    <t>001-003-013-1012-011-070-071</t>
-  </si>
-  <si>
-    <t>001-003-013-1012-011-070-068</t>
-  </si>
-  <si>
-    <t>001-003-013-1012-011-070</t>
-  </si>
-  <si>
-    <t>001-003-013-1012-011</t>
-  </si>
-  <si>
-    <t>001-003-013-012</t>
-  </si>
-  <si>
-    <t>001-003-013</t>
-  </si>
-  <si>
     <t>027-028-029-049-095-094</t>
   </si>
   <si>
@@ -18185,6 +18164,27 @@
   </si>
   <si>
     <t>032-027-028-029-049-095</t>
+  </si>
+  <si>
+    <t>001-1003-003-013-1012-011</t>
+  </si>
+  <si>
+    <t>001-1003-003-013-012</t>
+  </si>
+  <si>
+    <t>001-1003-003-013</t>
+  </si>
+  <si>
+    <t>001-1003-003-013-1012-011-070-068</t>
+  </si>
+  <si>
+    <t>001-1003-003-013-1012-011-070</t>
+  </si>
+  <si>
+    <t>001-1003-003-013-1012-011-070-071</t>
+  </si>
+  <si>
+    <t>001-1003-003-013-1012-011-070-071-073</t>
   </si>
 </sst>
 </file>
@@ -18536,8 +18536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7615"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A3054" workbookViewId="0">
+      <selection activeCell="B3066" sqref="B3066"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28213,7 +28213,7 @@
         <v>3604</v>
       </c>
       <c r="B882" t="s">
-        <v>6030</v>
+        <v>6023</v>
       </c>
       <c r="C882" t="s">
         <v>2296</v>
@@ -28224,7 +28224,7 @@
         <v>3605</v>
       </c>
       <c r="B883" t="s">
-        <v>6031</v>
+        <v>6024</v>
       </c>
       <c r="C883" t="s">
         <v>2296</v>
@@ -28796,7 +28796,7 @@
         <v>3666</v>
       </c>
       <c r="B935" t="s">
-        <v>6032</v>
+        <v>6025</v>
       </c>
       <c r="C935" t="s">
         <v>2296</v>
@@ -28807,7 +28807,7 @@
         <v>3667</v>
       </c>
       <c r="B936" t="s">
-        <v>6033</v>
+        <v>6026</v>
       </c>
       <c r="C936" t="s">
         <v>2296</v>
@@ -28884,7 +28884,7 @@
         <v>3730</v>
       </c>
       <c r="B943" t="s">
-        <v>6048</v>
+        <v>6041</v>
       </c>
       <c r="C943" t="s">
         <v>2296</v>
@@ -28939,7 +28939,7 @@
         <v>3735</v>
       </c>
       <c r="B948" t="s">
-        <v>6049</v>
+        <v>6042</v>
       </c>
       <c r="C948" t="s">
         <v>2296</v>
@@ -28950,7 +28950,7 @@
         <v>3736</v>
       </c>
       <c r="B949" t="s">
-        <v>6050</v>
+        <v>6043</v>
       </c>
       <c r="C949" t="s">
         <v>2296</v>
@@ -28961,7 +28961,7 @@
         <v>3737</v>
       </c>
       <c r="B950" t="s">
-        <v>6051</v>
+        <v>6044</v>
       </c>
       <c r="C950" t="s">
         <v>2296</v>
@@ -28972,7 +28972,7 @@
         <v>3738</v>
       </c>
       <c r="B951" t="s">
-        <v>6052</v>
+        <v>6045</v>
       </c>
       <c r="C951" t="s">
         <v>2296</v>
@@ -29093,7 +29093,7 @@
         <v>3700</v>
       </c>
       <c r="B962" t="s">
-        <v>6034</v>
+        <v>6027</v>
       </c>
       <c r="C962" t="s">
         <v>2296</v>
@@ -29104,7 +29104,7 @@
         <v>3701</v>
       </c>
       <c r="B963" t="s">
-        <v>6035</v>
+        <v>6028</v>
       </c>
       <c r="C963" t="s">
         <v>2296</v>
@@ -29170,7 +29170,7 @@
         <v>3708</v>
       </c>
       <c r="B969" t="s">
-        <v>6036</v>
+        <v>6029</v>
       </c>
       <c r="C969" t="s">
         <v>2296</v>
@@ -29181,7 +29181,7 @@
         <v>3709</v>
       </c>
       <c r="B970" t="s">
-        <v>6037</v>
+        <v>6030</v>
       </c>
       <c r="C970" t="s">
         <v>2296</v>
@@ -29192,7 +29192,7 @@
         <v>3710</v>
       </c>
       <c r="B971" t="s">
-        <v>6038</v>
+        <v>6031</v>
       </c>
       <c r="C971" t="s">
         <v>2296</v>
@@ -29214,7 +29214,7 @@
         <v>3711</v>
       </c>
       <c r="B973" t="s">
-        <v>6039</v>
+        <v>6032</v>
       </c>
       <c r="C973" t="s">
         <v>2296</v>
@@ -29225,7 +29225,7 @@
         <v>3712</v>
       </c>
       <c r="B974" t="s">
-        <v>6040</v>
+        <v>6033</v>
       </c>
       <c r="C974" t="s">
         <v>2296</v>
@@ -29236,7 +29236,7 @@
         <v>3713</v>
       </c>
       <c r="B975" t="s">
-        <v>6041</v>
+        <v>6034</v>
       </c>
       <c r="C975" t="s">
         <v>2296</v>
@@ -29280,7 +29280,7 @@
         <v>3714</v>
       </c>
       <c r="B979" t="s">
-        <v>6042</v>
+        <v>6035</v>
       </c>
       <c r="C979" t="s">
         <v>2296</v>
@@ -29445,7 +29445,7 @@
         <v>3725</v>
       </c>
       <c r="B994" t="s">
-        <v>6043</v>
+        <v>6036</v>
       </c>
       <c r="C994" t="s">
         <v>2296</v>
@@ -29456,7 +29456,7 @@
         <v>3726</v>
       </c>
       <c r="B995" t="s">
-        <v>6044</v>
+        <v>6037</v>
       </c>
       <c r="C995" t="s">
         <v>2296</v>
@@ -29467,7 +29467,7 @@
         <v>3727</v>
       </c>
       <c r="B996" t="s">
-        <v>6045</v>
+        <v>6038</v>
       </c>
       <c r="C996" t="s">
         <v>2296</v>
@@ -29489,7 +29489,7 @@
         <v>3728</v>
       </c>
       <c r="B998" t="s">
-        <v>6046</v>
+        <v>6039</v>
       </c>
       <c r="C998" t="s">
         <v>2296</v>
@@ -29500,7 +29500,7 @@
         <v>3729</v>
       </c>
       <c r="B999" t="s">
-        <v>6047</v>
+        <v>6040</v>
       </c>
       <c r="C999" t="s">
         <v>2296</v>
@@ -31106,7 +31106,7 @@
         <v>3869</v>
       </c>
       <c r="B1145" t="s">
-        <v>6053</v>
+        <v>6046</v>
       </c>
       <c r="C1145" t="s">
         <v>2296</v>
@@ -31304,7 +31304,7 @@
         <v>3882</v>
       </c>
       <c r="B1163" t="s">
-        <v>6054</v>
+        <v>6047</v>
       </c>
       <c r="C1163" t="s">
         <v>2296</v>
@@ -31315,7 +31315,7 @@
         <v>3883</v>
       </c>
       <c r="B1164" t="s">
-        <v>6055</v>
+        <v>6048</v>
       </c>
       <c r="C1164" t="s">
         <v>2296</v>
@@ -51201,7 +51201,7 @@
         <v>1207</v>
       </c>
       <c r="B2974" t="s">
-        <v>6027</v>
+        <v>6049</v>
       </c>
       <c r="C2974" t="s">
         <v>2298</v>
@@ -51300,7 +51300,7 @@
         <v>1211</v>
       </c>
       <c r="B2983" t="s">
-        <v>6028</v>
+        <v>6050</v>
       </c>
       <c r="C2983" t="s">
         <v>2298</v>
@@ -51311,7 +51311,7 @@
         <v>1210</v>
       </c>
       <c r="B2984" t="s">
-        <v>6029</v>
+        <v>6051</v>
       </c>
       <c r="C2984" t="s">
         <v>2298</v>
@@ -51641,7 +51641,7 @@
         <v>1201</v>
       </c>
       <c r="B3014" t="s">
-        <v>6025</v>
+        <v>6052</v>
       </c>
       <c r="C3014" t="s">
         <v>2298</v>
@@ -51663,7 +51663,7 @@
         <v>1206</v>
       </c>
       <c r="B3016" t="s">
-        <v>6026</v>
+        <v>6053</v>
       </c>
       <c r="C3016" t="s">
         <v>2298</v>
@@ -51674,7 +51674,7 @@
         <v>1204</v>
       </c>
       <c r="B3017" t="s">
-        <v>6024</v>
+        <v>6054</v>
       </c>
       <c r="C3017" t="s">
         <v>2298</v>
@@ -51729,7 +51729,7 @@
         <v>1200</v>
       </c>
       <c r="B3022" t="s">
-        <v>6023</v>
+        <v>6055</v>
       </c>
       <c r="C3022" t="s">
         <v>2298</v>

</xml_diff>

<commit_message>
Now if a path is not in the list provided by the user, it is automatically calculated using dijkstra. Rework builder methods for building a network with restricted links provided by the user.
</commit_message>
<xml_diff>
--- a/data/railway_paths.xlsx
+++ b/data/railway_paths.xlsx
@@ -18536,8 +18536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7615"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3054" workbookViewId="0">
-      <selection activeCell="B3066" sqref="B3066"/>
+    <sheetView tabSelected="1" topLeftCell="A3062" workbookViewId="0">
+      <selection activeCell="B3076" sqref="B3076"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>